<commit_message>
Testes e verificações quando Lista de Inputs ou Outputs esta vazia
</commit_message>
<xml_diff>
--- a/data/Dados.xlsx
+++ b/data/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="117">
   <si>
     <t>Ano</t>
   </si>
@@ -337,9 +337,6 @@
     <t>Pev_Obito</t>
   </si>
   <si>
-    <t>calcular_eventos_e_consequencias</t>
-  </si>
-  <si>
     <t>Nev_Afmenor15_Tipico</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>Nev_Obito_NRelac</t>
+  </si>
+  <si>
+    <t>calcular_eventos</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1503,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2367,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>85</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>86</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
         <v>87</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>88</v>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -2489,10 +2489,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -2501,10 +2501,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -2513,30 +2513,19 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2544,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,130 +2562,130 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>